<commit_message>
Added a few more cases to name search.  Pathogens now work for cdiff. Can handle blank rows now
</commit_message>
<xml_diff>
--- a/DataCleaning/mod_names.xlsx
+++ b/DataCleaning/mod_names.xlsx
@@ -15,48 +15,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Staff</t>
   </si>
   <si>
+    <t>Smith, J S P</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Smith, John</t>
+  </si>
+  <si>
     <t>Smith, John Samuel</t>
   </si>
   <si>
-    <t>Smith, John S.</t>
-  </si>
-  <si>
-    <t>Smith, John S</t>
-  </si>
-  <si>
     <t>Smith, J S</t>
   </si>
   <si>
     <t>Smith, J. S.</t>
   </si>
   <si>
-    <t>Smith, John</t>
-  </si>
-  <si>
-    <t>S., John</t>
-  </si>
-  <si>
-    <t>S, John</t>
-  </si>
-  <si>
-    <t>Smith, John Samuel Peter</t>
-  </si>
-  <si>
-    <t>Smith, John S P</t>
-  </si>
-  <si>
-    <t>Smith, J S P</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>Smith, John;Francis, Carol</t>
+  </si>
+  <si>
+    <t>Perone, Marti F</t>
+  </si>
+  <si>
+    <t>Cabot, E P</t>
+  </si>
+  <si>
+    <t>Mcfarland, Merralee Ives</t>
+  </si>
+  <si>
+    <t>Narayan, Rosalie</t>
+  </si>
+  <si>
+    <t>Takemoto, Roxie N</t>
+  </si>
+  <si>
+    <t>Schiada, T G</t>
+  </si>
+  <si>
+    <t>Fitzgibbon, Ginelle M</t>
+  </si>
+  <si>
+    <t>Teeven, Ninnetta J</t>
+  </si>
+  <si>
+    <t>Reinagle, Nessi</t>
+  </si>
+  <si>
+    <t>Cabot, Eolanda</t>
+  </si>
+  <si>
+    <t>Brecher, B</t>
+  </si>
+  <si>
+    <t>Pinero, Caril</t>
+  </si>
+  <si>
+    <t>Mcfarland, Merralee</t>
+  </si>
+  <si>
+    <t>Agresti, A</t>
+  </si>
+  <si>
+    <t>Hoppin, Sadye</t>
+  </si>
+  <si>
+    <t>Takemoto, Roxie</t>
+  </si>
+  <si>
+    <t>Styx, Lacy;Pope, Shanon;Seals, Amy;Dave, Marty</t>
+  </si>
+  <si>
+    <t>Park, Aaron</t>
+  </si>
+  <si>
+    <t>Madison., Madison Reel</t>
+  </si>
+  <si>
+    <t>Birch, Samuel;Thomas, Frieda</t>
+  </si>
+  <si>
+    <t>Douglas, Chris Mort;Cost,Allen</t>
+  </si>
+  <si>
+    <t>Iverson, Scott</t>
+  </si>
+  <si>
+    <t>Styx, Lacy;Pope, Shanon</t>
   </si>
 </sst>
 </file>
@@ -405,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,201 +464,239 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="n">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="n">
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="n">
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="n">
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="n">
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="n">
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="n">
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="n">
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="n">
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="n">
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="n">
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="n">
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="n">
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="n">
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="n">
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>13</v>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>